<commit_message>
Add introduction to this web application
</commit_message>
<xml_diff>
--- a/design/sites.xlsx
+++ b/design/sites.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="104">
   <si>
     <t>title</t>
   </si>
@@ -347,6 +347,15 @@
   </si>
   <si>
     <t>https://ejje.weblio.jp</t>
+  </si>
+  <si>
+    <t>https://tecadmin.net</t>
+  </si>
+  <si>
+    <t>https://ten-navi.com</t>
+  </si>
+  <si>
+    <t>http://nomad-salaryman.com</t>
   </si>
 </sst>
 </file>
@@ -724,7 +733,7 @@
   <dimension ref="A1:D123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.2"/>
@@ -1006,11 +1015,23 @@
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
+    <row r="26" spans="1:4">
+      <c r="B26" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
     <row r="27" spans="1:4">
       <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="B28" s="3" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="4"/>

</xml_diff>